<commit_message>
pdf support | material-wise-details | xlsx
</commit_message>
<xml_diff>
--- a/sample-companies.xlsx
+++ b/sample-companies.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -31,25 +31,52 @@
     <t xml:space="preserve">Address</t>
   </si>
   <si>
-    <t xml:space="preserve">India Construction Ltd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29ABCDE1234F1Z9</t>
+    <t xml:space="preserve">Contact Person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobile Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">America Construction Ltd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29ABCDE1234F1Z5</t>
   </si>
   <si>
     <t xml:space="preserve">123 Main Street, Mumbai, Maharashtra 400001</t>
   </si>
   <si>
-    <t xml:space="preserve">Canada Builders Pvt Ltd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30FGHIJ5678K2L1</t>
+    <t xml:space="preserve">Rajesh Kumar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9876543210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rajesh.kumar@abcconstruction.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Australia Builders Pvt Ltd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30FGHIJ5678K2L6</t>
   </si>
   <si>
     <t xml:space="preserve">456 Park Avenue, Delhi, Delhi 110001</t>
   </si>
   <si>
-    <t xml:space="preserve">America Materials Co</t>
+    <t xml:space="preserve">Priya Sharma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9876543211</t>
+  </si>
+  <si>
+    <t xml:space="preserve">priya.sharma@xyzbuilders.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canada Materials Co</t>
   </si>
   <si>
     <t xml:space="preserve">27KLMNO9012P3Q7</t>
@@ -58,19 +85,46 @@
     <t xml:space="preserve">789 Industrial Area, Bangalore, Karnataka 560001</t>
   </si>
   <si>
-    <t xml:space="preserve">Australia Suppliers</t>
+    <t xml:space="preserve">Amit Patel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9876543212</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amit.patel@defmaterials.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">India Suppliers</t>
   </si>
   <si>
     <t xml:space="preserve">321 Trade Center, Pune, Maharashtra 411001</t>
   </si>
   <si>
+    <t xml:space="preserve">Sneha Desai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9876543213</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sneha.desai@ghisuppliers.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">UK Enterprises</t>
   </si>
   <si>
-    <t xml:space="preserve">24RSTUV3456W4X4</t>
+    <t xml:space="preserve">24RSTUV3456W4X8</t>
   </si>
   <si>
     <t xml:space="preserve">654 Business Park, Hyderabad, Telangana 500001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vikram Singh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9876543214</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vikram.singh@jklenterprises.com</t>
   </si>
 </sst>
 </file>
@@ -168,16 +222,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -190,57 +243,111 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>11</v>
+        <v>20</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>13</v>
+        <v>25</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>16</v>
+        <v>31</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>